<commit_message>
Concatenate author names to single entry string
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>ORESU-E-20-007</t>
   </si>
@@ -25,13 +25,7 @@
     <t>Oyster Larvae Catastrophe: What caused the oyster larvae die off, and what can we do?</t>
   </si>
   <si>
-    <t>Johnson, William</t>
-  </si>
-  <si>
-    <t>Wacker, Heidi</t>
-  </si>
-  <si>
-    <t>Calvanese, Tom</t>
+    <t>Johnson, William; Wacker, Heidi; Calvanese, Tom</t>
   </si>
   <si>
     <t>2020</t>
@@ -378,13 +372,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:M3"/>
+  <dimension ref="A3:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -401,28 +395,22 @@
         <v>4</v>
       </c>
       <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
         <v>5</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>6</v>
       </c>
-      <c r="H3" t="s">
-        <v>1</v>
-      </c>
       <c r="I3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
         <v>7</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>8</v>
-      </c>
-      <c r="K3" t="s">
-        <v>0</v>
-      </c>
-      <c r="L3" t="s">
-        <v>9</v>
-      </c>
-      <c r="M3" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>